<commit_message>
walkthrough videos and formative report
</commit_message>
<xml_diff>
--- a/docs/data/demo.xlsx
+++ b/docs/data/demo.xlsx
@@ -433,7 +433,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>44634</v>
+        <v>44636</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>44633</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>44632</v>
+        <v>44634</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44631</v>
+        <v>44633</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +511,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="1" t="n">
-        <v>44630</v>
+        <v>44632</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>44629</v>
+        <v>44631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>